<commit_message>
Add final PSNR results to repo
</commit_message>
<xml_diff>
--- a/psnr/psnrs.xlsx
+++ b/psnr/psnrs.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -606,7 +606,50 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1090,7 +1133,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -1164,11 +1207,108 @@
     </i>
   </colItems>
   <pageFields count="1">
-    <pageField fld="1" item="0" hier="-1"/>
+    <pageField fld="1" item="3" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Max of PSNR" fld="3" subtotal="max" baseField="0" baseItem="0"/>
+    <dataField name="Max of PSNR" fld="3" subtotal="max" baseField="0" baseItem="2"/>
   </dataFields>
+  <conditionalFormats count="5">
+    <conditionalFormat priority="5">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="3">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="4">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="3">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="3">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="3">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="3">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="3">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -1444,14 +1584,14 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F5" sqref="F5:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="6" customWidth="1"/>
+    <col min="3" max="6" width="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1460,7 +1600,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1499,22 +1639,22 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>32.979999999999997</v>
+        <v>20.78</v>
       </c>
       <c r="C5" s="1">
-        <v>32.65</v>
+        <v>17.82</v>
       </c>
       <c r="D5" s="1">
-        <v>31.59</v>
+        <v>15.65</v>
       </c>
       <c r="E5" s="1">
-        <v>30.91</v>
+        <v>14.36</v>
       </c>
       <c r="F5" s="1">
-        <v>30.36</v>
+        <v>13.55</v>
       </c>
       <c r="G5" s="1">
-        <v>32.979999999999997</v>
+        <v>20.78</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1522,22 +1662,22 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>36.72</v>
+        <v>25.98</v>
       </c>
       <c r="C6" s="1">
-        <v>34.15</v>
+        <v>21.85</v>
       </c>
       <c r="D6" s="1">
-        <v>32.979999999999997</v>
+        <v>18.62</v>
       </c>
       <c r="E6" s="1">
-        <v>32.26</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="F6" s="1">
-        <v>31.73</v>
+        <v>14.99</v>
       </c>
       <c r="G6" s="1">
-        <v>36.72</v>
+        <v>25.98</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1545,22 +1685,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>37.159999999999997</v>
+        <v>27.03</v>
       </c>
       <c r="C7" s="1">
-        <v>34.07</v>
+        <v>21.74</v>
       </c>
       <c r="D7" s="1">
-        <v>32.96</v>
+        <v>18.55</v>
       </c>
       <c r="E7" s="1">
-        <v>32.26</v>
+        <v>16.39</v>
       </c>
       <c r="F7" s="1">
-        <v>31.73</v>
+        <v>15.02</v>
       </c>
       <c r="G7" s="1">
-        <v>37.159999999999997</v>
+        <v>27.03</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1568,26 +1708,52 @@
         <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>37.159999999999997</v>
+        <v>27.03</v>
       </c>
       <c r="C8" s="1">
-        <v>34.15</v>
+        <v>21.85</v>
       </c>
       <c r="D8" s="1">
-        <v>32.979999999999997</v>
+        <v>18.62</v>
       </c>
       <c r="E8" s="1">
-        <v>32.26</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="F8" s="1">
-        <v>31.73</v>
+        <v>15.02</v>
       </c>
       <c r="G8" s="1">
-        <v>37.159999999999997</v>
+        <v>27.03</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting pivot="1" sqref="B5:B7">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>$B5=MAX($B$5:$B$7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="C5:C7">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>C5=MAX(C5:C7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="D5:D7">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>D5=MAX(D5:D7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="E5:E7">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>E5=MAX(E5:E7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="F5:F7">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>F5=MAX(F5:F7)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1595,7 +1761,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>